<commit_message>
Added line page (working)
</commit_message>
<xml_diff>
--- a/Goal-IEEE-13BUS.xlsx
+++ b/Goal-IEEE-13BUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbcloud-my.sharepoint.com/personal/ebelliv1_unb_ca/Documents/Smart Grid/Github/CYME-EXTRACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7538F9C7-4528-44E2-A2DB-56BFF7E84195}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{065897D2-71D8-4A61-BFDA-EF5FC7CD5317}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="932" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="15" r:id="rId1"/>
@@ -2059,10 +2059,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="34" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -3871,48 +3871,48 @@
     </row>
     <row r="7" spans="1:8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="9" t="s">
         <v>184</v>
       </c>
@@ -3938,21 +3938,21 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="9" t="s">
         <v>184</v>
       </c>
@@ -3979,21 +3979,21 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="9" t="s">
         <v>184</v>
       </c>
@@ -4055,21 +4055,21 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="9" t="s">
         <v>184</v>
       </c>
@@ -4107,12 +4107,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4127,17 +4127,17 @@
     <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Voltage Source'!positivesequence" display="PositiveSequence" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -4159,8 +4159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4219,40 +4219,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -4281,11 +4281,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="15" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -4598,10 +4598,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B30" s="22"/>
+      <c r="B30" s="21"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4968,6 +4968,11 @@
     <protectedRange sqref="D14:E14 A14 D17:E18 A17:A18 D21:E21 A21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="15">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A36:B36"/>
@@ -4978,11 +4983,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Load!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -5007,7 +5007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5015,6 +5017,7 @@
     <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5056,40 +5059,40 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6019,6 +6022,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A19:B19"/>
@@ -6027,11 +6035,6 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Line!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -6110,40 +6113,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6627,17 +6630,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Transformer!PostiveSequence2W" display="PositiveSequence2WTransformer" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -6714,40 +6717,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6998,17 +7001,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Shunt!positivesequence" display="PositiveSequenceShunt" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
@@ -7029,9 +7032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Checkpoint, now removing '-'
</commit_message>
<xml_diff>
--- a/Goal-IEEE-13BUS.xlsx
+++ b/Goal-IEEE-13BUS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C39D82-0E48-477A-B074-9D5DC82BF86C}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="932" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="15" r:id="rId1"/>
@@ -2059,10 +2059,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="34" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -2122,6 +2122,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3821,7 +3825,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3871,48 +3875,48 @@
     </row>
     <row r="7" spans="1:8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="9" t="s">
         <v>184</v>
       </c>
@@ -3938,21 +3942,21 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="9" t="s">
         <v>184</v>
       </c>
@@ -3979,21 +3983,21 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="9" t="s">
         <v>184</v>
       </c>
@@ -4055,21 +4059,21 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="9" t="s">
         <v>184</v>
       </c>
@@ -4107,12 +4111,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4127,17 +4131,17 @@
     <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Voltage Source'!positivesequence" display="PositiveSequence" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -4159,7 +4163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
@@ -4219,40 +4223,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -4281,11 +4285,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
     </row>
     <row r="15" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -4598,10 +4602,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B30" s="21"/>
+      <c r="B30" s="22"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4968,11 +4972,6 @@
     <protectedRange sqref="D14:E14 A14 D17:E18 A17:A18 D21:E21 A21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="15">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A36:B36"/>
@@ -4983,6 +4982,11 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Load!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -5059,40 +5063,40 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6022,11 +6026,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A19:B19"/>
@@ -6035,6 +6034,11 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Line!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -6115,40 +6119,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6632,17 +6636,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Transformer!PostiveSequence2W" display="PositiveSequence2WTransformer" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -6663,8 +6667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:N27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6721,40 +6725,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -7005,17 +7009,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Shunt!positivesequence" display="PositiveSequenceShunt" xr:uid="{00000000-0004-0000-0700-000000000000}"/>

</xml_diff>

<commit_message>
Working with CYME 34BUS
</commit_message>
<xml_diff>
--- a/Goal-IEEE-13BUS.xlsx
+++ b/Goal-IEEE-13BUS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C39D82-0E48-477A-B074-9D5DC82BF86C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="932" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="15" r:id="rId1"/>
@@ -2059,10 +2059,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="34" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -2466,7 +2466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3875,48 +3875,48 @@
     </row>
     <row r="7" spans="1:8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="9" t="s">
         <v>184</v>
       </c>
@@ -3942,21 +3942,21 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="9" t="s">
         <v>184</v>
       </c>
@@ -3983,21 +3983,21 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="9" t="s">
         <v>184</v>
       </c>
@@ -4059,21 +4059,21 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="9" t="s">
         <v>184</v>
       </c>
@@ -4111,12 +4111,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4131,17 +4131,17 @@
     <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Voltage Source'!positivesequence" display="PositiveSequence" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -4163,7 +4163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
@@ -4223,40 +4223,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -4285,11 +4285,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="15" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -4602,10 +4602,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B30" s="22"/>
+      <c r="B30" s="21"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4972,6 +4972,11 @@
     <protectedRange sqref="D14:E14 A14 D17:E18 A17:A18 D21:E21 A21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="15">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A36:B36"/>
@@ -4982,11 +4987,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Load!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -5063,40 +5063,40 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6026,6 +6026,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A19:B19"/>
@@ -6034,11 +6039,6 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Line!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -6061,7 +6061,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6119,40 +6119,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6636,17 +6636,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Transformer!PostiveSequence2W" display="PositiveSequence2WTransformer" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -6668,7 +6668,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6725,40 +6725,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -7009,17 +7009,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Shunt!positivesequence" display="PositiveSequenceShunt" xr:uid="{00000000-0004-0000-0700-000000000000}"/>

</xml_diff>

<commit_message>
Working on full sim (needs one source only)
</commit_message>
<xml_diff>
--- a/Goal-IEEE-13BUS.xlsx
+++ b/Goal-IEEE-13BUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbcloud-my.sharepoint.com/personal/ebelliv1_unb_ca/Documents/Smart Grid/Github/CYME-EXTRACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C39D82-0E48-477A-B074-9D5DC82BF86C}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{F89594DD-2510-4F7D-87A7-FB396182D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F2870C9-EEA2-47D3-A2B5-EB8FE72C2D72}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="932" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="932" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="15" r:id="rId1"/>
@@ -2059,10 +2059,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="34" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -2466,7 +2466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3875,48 +3875,48 @@
     </row>
     <row r="7" spans="1:8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="9" t="s">
         <v>184</v>
       </c>
@@ -3942,21 +3942,21 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="9" t="s">
         <v>184</v>
       </c>
@@ -3983,21 +3983,21 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="9" t="s">
         <v>184</v>
       </c>
@@ -4059,21 +4059,21 @@
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="9" t="s">
         <v>184</v>
       </c>
@@ -4111,12 +4111,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4131,17 +4131,17 @@
     <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Voltage Source'!positivesequence" display="PositiveSequence" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -4223,40 +4223,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -4285,11 +4285,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
     </row>
     <row r="15" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -4602,10 +4602,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B30" s="21"/>
+      <c r="B30" s="22"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4972,11 +4972,6 @@
     <protectedRange sqref="D14:E14 A14 D17:E18 A17:A18 D21:E21 A21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="15">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A36:B36"/>
@@ -4987,6 +4982,11 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Load!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -5012,7 +5012,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5063,40 +5063,40 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6026,11 +6026,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A19:B19"/>
@@ -6039,6 +6034,11 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" location="Line!Type" display="Go to Type List" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -6060,8 +6060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6072,6 +6072,7 @@
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6119,40 +6120,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -6636,17 +6637,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Transformer!PostiveSequence2W" display="PositiveSequence2WTransformer" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -6725,40 +6726,40 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -7009,17 +7010,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Shunt!positivesequence" display="PositiveSequenceShunt" xr:uid="{00000000-0004-0000-0700-000000000000}"/>

</xml_diff>